<commit_message>
unpredictable worse situation, better collision avoidance need to be considered
</commit_message>
<xml_diff>
--- a/ILP/comparison.xlsx
+++ b/ILP/comparison.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1759921\Documents\code\matlab\Neural-Networks\ILP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D5AF913-63C9-45BA-90B4-380DF5998C6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67C4978-18D5-4FB0-887D-7FB1A408DA2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4970"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t># of correct labels</t>
   </si>
@@ -54,12 +55,42 @@
   </si>
   <si>
     <t>irregular + no mapping</t>
+  </si>
+  <si>
+    <t>flow 10</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>flow 20</t>
+  </si>
+  <si>
+    <t>MILP</t>
+  </si>
+  <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>GCA</t>
+  </si>
+  <si>
+    <t>GRC</t>
+  </si>
+  <si>
+    <t>storage invalidation</t>
+  </si>
+  <si>
+    <t>link capacity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,9 +120,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,11 +448,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,4 +723,280 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC7A513-A556-4771-974F-7C92905D56A5}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8.2609999999999992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>10.879</v>
+      </c>
+      <c r="C3" s="2">
+        <v>11.327</v>
+      </c>
+      <c r="D3" s="2">
+        <v>15.618</v>
+      </c>
+      <c r="E3" s="2">
+        <v>11.201000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.97309999999999997</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.76419999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.74660000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.86750000000000005</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6.0499999999999998E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>6.0499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.988</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9.3510000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
+        <v>22.061</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44.923999999999999</v>
+      </c>
+      <c r="D11" s="2">
+        <v>74.236999999999995</v>
+      </c>
+      <c r="E11" s="2">
+        <v>45.601999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.65690000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="D14" s="3">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.42449999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C16" s="4">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="2">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2">
+        <v>1145</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>